<commit_message>
update tags and description
</commit_message>
<xml_diff>
--- a/tables/nomenclature/petri-placestransitions.xlsx
+++ b/tables/nomenclature/petri-placestransitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Accacio\Documents\docsTCC\tables\nomenclature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E04AF6-22FF-49B2-AB0D-87BE3C5F339B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0847D26C-FA04-4C5C-BB2F-7F053126F313}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="11385" xr2:uid="{E999CB99-BFAE-438B-9F43-BAC24AB08F3B}"/>
+    <workbookView xWindow="3120" yWindow="2490" windowWidth="28800" windowHeight="12015" xr2:uid="{E999CB99-BFAE-438B-9F43-BAC24AB08F3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -453,24 +453,6 @@
     <t>p139</t>
   </si>
   <si>
-    <t>p140</t>
-  </si>
-  <si>
-    <t>p141</t>
-  </si>
-  <si>
-    <t>p142</t>
-  </si>
-  <si>
-    <t>p143</t>
-  </si>
-  <si>
-    <t>p144</t>
-  </si>
-  <si>
-    <t>p145</t>
-  </si>
-  <si>
     <t>PLC2</t>
   </si>
   <si>
@@ -1384,6 +1366,24 @@
   </si>
   <si>
     <t>b149</t>
+  </si>
+  <si>
+    <t>t150</t>
+  </si>
+  <si>
+    <t>t152</t>
+  </si>
+  <si>
+    <t>t151</t>
+  </si>
+  <si>
+    <t>b150</t>
+  </si>
+  <si>
+    <t>b151</t>
+  </si>
+  <si>
+    <t>b152</t>
   </si>
 </sst>
 </file>
@@ -1738,10 +1738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9FAA90E-D89F-4CC1-AE78-0A03061E385F}">
-  <dimension ref="A1:I90"/>
+  <dimension ref="A1:I93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="G82" sqref="G82:G87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1754,26 +1754,26 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B1" s="1"/>
       <c r="G1" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="G2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="H2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1781,19 +1781,19 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C3" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="G3" t="s">
         <v>14</v>
       </c>
       <c r="H3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="I3" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1801,19 +1801,19 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C4" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="G4" t="s">
         <v>15</v>
       </c>
       <c r="H4" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="I4" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1821,19 +1821,19 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C5" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="G5" t="s">
         <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="I5" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1841,19 +1841,19 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C6" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="G6" t="s">
         <v>17</v>
       </c>
       <c r="H6" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="I6" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1861,19 +1861,19 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C7" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="G7" t="s">
         <v>18</v>
       </c>
       <c r="H7" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I7" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1881,19 +1881,19 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C8" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="G8" t="s">
         <v>19</v>
       </c>
       <c r="H8" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I8" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1901,19 +1901,19 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C9" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="G9" t="s">
         <v>20</v>
       </c>
       <c r="H9" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I9" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1921,19 +1921,19 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C10" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="G10" t="s">
         <v>21</v>
       </c>
       <c r="H10" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="I10" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1941,19 +1941,19 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C11" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="G11" t="s">
         <v>22</v>
       </c>
       <c r="H11" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="I11" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1961,19 +1961,19 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C12" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="G12" t="s">
         <v>23</v>
       </c>
       <c r="H12" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="I12" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1981,19 +1981,19 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C13" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="G13" t="s">
         <v>24</v>
       </c>
       <c r="H13" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="I13" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2001,19 +2001,19 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C14" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="G14" t="s">
         <v>25</v>
       </c>
       <c r="H14" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="I14" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2021,19 +2021,19 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C15" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="G15" t="s">
         <v>26</v>
       </c>
       <c r="H15" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="I15" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2041,19 +2041,19 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C16" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="G16" t="s">
         <v>74</v>
       </c>
       <c r="H16" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="I16" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2061,19 +2061,19 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C17" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="G17" t="s">
         <v>75</v>
       </c>
       <c r="H17" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="I17" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -2081,19 +2081,19 @@
         <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C18" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="G18" t="s">
         <v>76</v>
       </c>
       <c r="H18" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="I18" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2101,19 +2101,19 @@
         <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="C19" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="G19" t="s">
         <v>77</v>
       </c>
       <c r="H19" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="I19" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -2121,19 +2121,19 @@
         <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="C20" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="G20" t="s">
         <v>78</v>
       </c>
       <c r="H20" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="I20" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -2141,19 +2141,19 @@
         <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C21" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="G21" t="s">
         <v>79</v>
       </c>
       <c r="H21" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="I21" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2161,19 +2161,19 @@
         <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="C22" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G22" t="s">
         <v>80</v>
       </c>
       <c r="H22" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="I22" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -2181,19 +2181,19 @@
         <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C23" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="G23" t="s">
         <v>81</v>
       </c>
       <c r="H23" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="I23" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -2201,19 +2201,19 @@
         <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C24" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="G24" t="s">
         <v>82</v>
       </c>
       <c r="H24" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="I24" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -2221,19 +2221,19 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C25" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="G25" t="s">
         <v>83</v>
       </c>
       <c r="H25" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="I25" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -2241,19 +2241,19 @@
         <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C26" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="G26" t="s">
         <v>84</v>
       </c>
       <c r="H26" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="I26" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -2261,19 +2261,19 @@
         <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C27" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="G27" t="s">
         <v>85</v>
       </c>
       <c r="H27" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="I27" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -2281,19 +2281,19 @@
         <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="C28" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="G28" t="s">
         <v>86</v>
       </c>
       <c r="H28" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="I28" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -2301,19 +2301,19 @@
         <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C29" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="G29" t="s">
         <v>87</v>
       </c>
       <c r="H29" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="I29" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2321,19 +2321,19 @@
         <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C30" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="G30" t="s">
         <v>88</v>
       </c>
       <c r="H30" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="I30" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -2341,19 +2341,19 @@
         <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C31" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="G31" t="s">
         <v>89</v>
       </c>
       <c r="H31" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="I31" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -2361,19 +2361,19 @@
         <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C32" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="G32" t="s">
         <v>90</v>
       </c>
       <c r="H32" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="I32" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -2381,19 +2381,19 @@
         <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C33" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="G33" t="s">
         <v>91</v>
       </c>
       <c r="H33" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="I33" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -2401,19 +2401,19 @@
         <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="C34" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="G34" t="s">
         <v>92</v>
       </c>
       <c r="H34" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="I34" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2421,19 +2421,19 @@
         <v>45</v>
       </c>
       <c r="B35" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C35" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="G35" t="s">
         <v>93</v>
       </c>
       <c r="H35" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="I35" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -2441,19 +2441,19 @@
         <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C36" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="G36" t="s">
         <v>94</v>
       </c>
       <c r="H36" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="I36" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2461,19 +2461,19 @@
         <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C37" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="G37" t="s">
         <v>95</v>
       </c>
       <c r="H37" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="I37" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2481,19 +2481,19 @@
         <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C38" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="G38" t="s">
         <v>96</v>
       </c>
       <c r="H38" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="I38" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2501,19 +2501,19 @@
         <v>49</v>
       </c>
       <c r="B39" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="C39" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="G39" t="s">
         <v>97</v>
       </c>
       <c r="H39" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="I39" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2521,19 +2521,19 @@
         <v>50</v>
       </c>
       <c r="B40" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C40" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="G40" t="s">
         <v>98</v>
       </c>
       <c r="H40" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I40" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2541,19 +2541,19 @@
         <v>51</v>
       </c>
       <c r="B41" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C41" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="G41" t="s">
         <v>99</v>
       </c>
       <c r="H41" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="I41" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -2561,19 +2561,19 @@
         <v>52</v>
       </c>
       <c r="B42" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C42" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="G42" t="s">
         <v>100</v>
       </c>
       <c r="H42" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="I42" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -2581,19 +2581,19 @@
         <v>53</v>
       </c>
       <c r="B43" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C43" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="G43" t="s">
         <v>101</v>
       </c>
       <c r="H43" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="I43" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -2601,19 +2601,19 @@
         <v>54</v>
       </c>
       <c r="B44" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C44" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="G44" t="s">
         <v>102</v>
       </c>
       <c r="H44" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="I44" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -2621,19 +2621,19 @@
         <v>55</v>
       </c>
       <c r="B45" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C45" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="G45" t="s">
         <v>103</v>
       </c>
       <c r="H45" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="I45" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -2641,19 +2641,19 @@
         <v>56</v>
       </c>
       <c r="B46" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C46" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="G46" t="s">
         <v>104</v>
       </c>
       <c r="H46" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="I46" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -2661,19 +2661,19 @@
         <v>57</v>
       </c>
       <c r="B47" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C47" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="G47" t="s">
         <v>105</v>
       </c>
       <c r="H47" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="I47" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2681,19 +2681,19 @@
         <v>58</v>
       </c>
       <c r="B48" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C48" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="G48" t="s">
         <v>106</v>
       </c>
       <c r="H48" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="I48" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -2701,19 +2701,19 @@
         <v>59</v>
       </c>
       <c r="B49" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C49" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="G49" t="s">
         <v>107</v>
       </c>
       <c r="H49" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="I49" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -2721,19 +2721,19 @@
         <v>60</v>
       </c>
       <c r="B50" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C50" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="G50" t="s">
         <v>108</v>
       </c>
       <c r="H50" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="I50" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -2741,19 +2741,19 @@
         <v>61</v>
       </c>
       <c r="B51" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C51" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="G51" t="s">
         <v>109</v>
       </c>
       <c r="H51" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="I51" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -2761,19 +2761,19 @@
         <v>62</v>
       </c>
       <c r="B52" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C52" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="G52" t="s">
         <v>110</v>
       </c>
       <c r="H52" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="I52" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2781,19 +2781,19 @@
         <v>63</v>
       </c>
       <c r="B53" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C53" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="G53" t="s">
         <v>111</v>
       </c>
       <c r="H53" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="I53" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -2801,19 +2801,19 @@
         <v>64</v>
       </c>
       <c r="B54" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="C54" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="G54" t="s">
         <v>112</v>
       </c>
       <c r="H54" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="I54" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -2821,19 +2821,19 @@
         <v>65</v>
       </c>
       <c r="B55" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C55" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="G55" t="s">
         <v>113</v>
       </c>
       <c r="H55" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="I55" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -2841,19 +2841,19 @@
         <v>66</v>
       </c>
       <c r="B56" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C56" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="G56" t="s">
         <v>114</v>
       </c>
       <c r="H56" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="I56" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2861,19 +2861,19 @@
         <v>67</v>
       </c>
       <c r="B57" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C57" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="G57" t="s">
         <v>115</v>
       </c>
       <c r="H57" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="I57" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -2881,19 +2881,19 @@
         <v>68</v>
       </c>
       <c r="B58" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="C58" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="G58" t="s">
         <v>116</v>
       </c>
       <c r="H58" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="I58" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -2901,19 +2901,19 @@
         <v>69</v>
       </c>
       <c r="B59" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C59" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="G59" t="s">
         <v>117</v>
       </c>
       <c r="H59" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="I59" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -2921,19 +2921,19 @@
         <v>70</v>
       </c>
       <c r="B60" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C60" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="G60" t="s">
         <v>118</v>
       </c>
       <c r="H60" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="I60" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -2941,19 +2941,19 @@
         <v>71</v>
       </c>
       <c r="B61" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="C61" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="G61" t="s">
         <v>119</v>
       </c>
       <c r="H61" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="I61" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -2961,19 +2961,19 @@
         <v>72</v>
       </c>
       <c r="B62" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C62" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="G62" t="s">
         <v>120</v>
       </c>
       <c r="H62" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="I62" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -2981,36 +2981,36 @@
         <v>73</v>
       </c>
       <c r="B63" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="C63" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="G63" t="s">
         <v>121</v>
       </c>
       <c r="H63" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="I63" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C64" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="G64" t="s">
         <v>122</v>
       </c>
       <c r="H64" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="I64" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
     </row>
     <row r="65" spans="7:9" x14ac:dyDescent="0.25">
@@ -3018,10 +3018,10 @@
         <v>123</v>
       </c>
       <c r="H65" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="I65" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
     </row>
     <row r="66" spans="7:9" x14ac:dyDescent="0.25">
@@ -3029,10 +3029,10 @@
         <v>124</v>
       </c>
       <c r="H66" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="I66" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
     </row>
     <row r="67" spans="7:9" x14ac:dyDescent="0.25">
@@ -3040,10 +3040,10 @@
         <v>125</v>
       </c>
       <c r="H67" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="I67" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
     </row>
     <row r="68" spans="7:9" x14ac:dyDescent="0.25">
@@ -3051,10 +3051,10 @@
         <v>126</v>
       </c>
       <c r="H68" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="I68" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
     </row>
     <row r="69" spans="7:9" x14ac:dyDescent="0.25">
@@ -3062,10 +3062,10 @@
         <v>127</v>
       </c>
       <c r="H69" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="I69" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
     </row>
     <row r="70" spans="7:9" x14ac:dyDescent="0.25">
@@ -3073,10 +3073,10 @@
         <v>128</v>
       </c>
       <c r="H70" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="I70" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
     </row>
     <row r="71" spans="7:9" x14ac:dyDescent="0.25">
@@ -3084,10 +3084,10 @@
         <v>129</v>
       </c>
       <c r="H71" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="I71" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
     </row>
     <row r="72" spans="7:9" x14ac:dyDescent="0.25">
@@ -3095,10 +3095,10 @@
         <v>130</v>
       </c>
       <c r="H72" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="I72" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
     </row>
     <row r="73" spans="7:9" x14ac:dyDescent="0.25">
@@ -3106,10 +3106,10 @@
         <v>131</v>
       </c>
       <c r="H73" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="I73" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
     </row>
     <row r="74" spans="7:9" x14ac:dyDescent="0.25">
@@ -3117,10 +3117,10 @@
         <v>132</v>
       </c>
       <c r="H74" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="I74" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
     </row>
     <row r="75" spans="7:9" x14ac:dyDescent="0.25">
@@ -3128,10 +3128,10 @@
         <v>133</v>
       </c>
       <c r="H75" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="I75" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
     </row>
     <row r="76" spans="7:9" x14ac:dyDescent="0.25">
@@ -3139,10 +3139,10 @@
         <v>134</v>
       </c>
       <c r="H76" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="I76" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
     </row>
     <row r="77" spans="7:9" x14ac:dyDescent="0.25">
@@ -3150,10 +3150,10 @@
         <v>135</v>
       </c>
       <c r="H77" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="I77" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
     </row>
     <row r="78" spans="7:9" x14ac:dyDescent="0.25">
@@ -3161,10 +3161,10 @@
         <v>136</v>
       </c>
       <c r="H78" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="I78" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
     </row>
     <row r="79" spans="7:9" x14ac:dyDescent="0.25">
@@ -3172,10 +3172,10 @@
         <v>137</v>
       </c>
       <c r="H79" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="I79" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
     </row>
     <row r="80" spans="7:9" x14ac:dyDescent="0.25">
@@ -3183,10 +3183,10 @@
         <v>138</v>
       </c>
       <c r="H80" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="I80" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
     </row>
     <row r="81" spans="7:9" x14ac:dyDescent="0.25">
@@ -3194,99 +3194,105 @@
         <v>139</v>
       </c>
       <c r="H81" t="s">
+        <v>285</v>
+      </c>
+      <c r="I81" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="82" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="H82" t="s">
+        <v>286</v>
+      </c>
+      <c r="I82" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="83" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="H83" t="s">
+        <v>287</v>
+      </c>
+      <c r="I83" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="84" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="H84" t="s">
+        <v>288</v>
+      </c>
+      <c r="I84" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="85" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="H85" t="s">
+        <v>289</v>
+      </c>
+      <c r="I85" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="86" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="H86" t="s">
+        <v>290</v>
+      </c>
+      <c r="I86" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="87" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="H87" t="s">
         <v>291</v>
       </c>
-      <c r="I81" t="s">
+      <c r="I87" t="s">
         <v>441</v>
-      </c>
-    </row>
-    <row r="82" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G82" t="s">
-        <v>140</v>
-      </c>
-      <c r="H82" t="s">
-        <v>292</v>
-      </c>
-      <c r="I82" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="83" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G83" t="s">
-        <v>141</v>
-      </c>
-      <c r="H83" t="s">
-        <v>293</v>
-      </c>
-      <c r="I83" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="84" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G84" t="s">
-        <v>142</v>
-      </c>
-      <c r="H84" t="s">
-        <v>294</v>
-      </c>
-      <c r="I84" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="85" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G85" t="s">
-        <v>143</v>
-      </c>
-      <c r="H85" t="s">
-        <v>295</v>
-      </c>
-      <c r="I85" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="86" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G86" t="s">
-        <v>144</v>
-      </c>
-      <c r="H86" t="s">
-        <v>296</v>
-      </c>
-      <c r="I86" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="87" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G87" t="s">
-        <v>145</v>
-      </c>
-      <c r="H87" t="s">
-        <v>297</v>
-      </c>
-      <c r="I87" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="88" spans="7:9" x14ac:dyDescent="0.25">
       <c r="H88" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="I88" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
     </row>
     <row r="89" spans="7:9" x14ac:dyDescent="0.25">
       <c r="H89" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="I89" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
     </row>
     <row r="90" spans="7:9" x14ac:dyDescent="0.25">
       <c r="H90" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="I90" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="91" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="H91" t="s">
+        <v>445</v>
+      </c>
+      <c r="I91" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="92" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="H92" t="s">
+        <v>447</v>
+      </c>
+      <c r="I92" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="93" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="H93" t="s">
+        <v>446</v>
+      </c>
+      <c r="I93" t="s">
         <v>450</v>
       </c>
     </row>

</xml_diff>